<commit_message>
Done tự động generate khám bệnh + Kê toa
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Thuốc.xlsx
+++ b/DataTest/Data_API_Thuốc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DS6"/>
+  <dimension ref="A1:DS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1792,1119 +1792,6 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3839</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" t="n">
-        <v>17437</v>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Quách Bảo Hưng</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="n">
-        <v>4803</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>knt1</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>13</v>
-      </c>
-      <c r="T4" t="n">
-        <v>13</v>
-      </c>
-      <c r="U4" t="n">
-        <v>30</v>
-      </c>
-      <c r="V4" t="n">
-        <v>130</v>
-      </c>
-      <c r="W4" t="n">
-        <v>2</v>
-      </c>
-      <c r="X4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Lần</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>Khám Nội Tiết 1</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Khám Nội tiết</t>
-        </is>
-      </c>
-      <c r="AB4" t="n">
-        <v>1024</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>7.1897</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>1083660</v>
-      </c>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>17437|983307|149|10/05/2024 01:02|A00.9|Bệnh tả, không đặc hiệu|3839|3|10/05/2024 01:02|3839||||PendingProcessing|4803|80||Bệnh tả, không đặc hiệu|2|1083660|13||</t>
-        </is>
-      </c>
-      <c r="AL4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>28</v>
-      </c>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="n">
-        <v>9843</v>
-      </c>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV4" t="inlineStr"/>
-      <c r="AW4" t="inlineStr"/>
-      <c r="AX4" t="inlineStr"/>
-      <c r="AY4" t="inlineStr"/>
-      <c r="AZ4" t="inlineStr"/>
-      <c r="BA4" t="inlineStr"/>
-      <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150) 150mg</t>
-        </is>
-      </c>
-      <c r="BD4" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="BE4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BF4" t="inlineStr"/>
-      <c r="BG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BI4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>127</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>5</v>
-      </c>
-      <c r="BN4" t="b">
-        <v>0</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP4" t="inlineStr">
-        <is>
-          <t>150mg</t>
-        </is>
-      </c>
-      <c r="BQ4" t="inlineStr">
-        <is>
-          <t>Uống</t>
-        </is>
-      </c>
-      <c r="BR4" t="inlineStr"/>
-      <c r="BS4" t="inlineStr">
-        <is>
-          <t>IrbT26</t>
-        </is>
-      </c>
-      <c r="BT4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU4" t="n">
-        <v>43</v>
-      </c>
-      <c r="BV4" t="inlineStr"/>
-      <c r="BW4" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150)</t>
-        </is>
-      </c>
-      <c r="BX4" t="inlineStr"/>
-      <c r="BY4" t="n">
-        <v>40.506</v>
-      </c>
-      <c r="BZ4" t="inlineStr">
-        <is>
-          <t>Hatlop-150</t>
-        </is>
-      </c>
-      <c r="CA4" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="CB4" t="inlineStr">
-        <is>
-          <t>Hộp</t>
-        </is>
-      </c>
-      <c r="CC4" t="inlineStr">
-        <is>
-          <t>Hộp</t>
-        </is>
-      </c>
-      <c r="CD4" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="CE4" t="n">
-        <v>100</v>
-      </c>
-      <c r="CF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CG4" t="inlineStr">
-        <is>
-          <t>Irbesartan</t>
-        </is>
-      </c>
-      <c r="CH4" t="n">
-        <v>101</v>
-      </c>
-      <c r="CI4" t="n">
-        <v>101</v>
-      </c>
-      <c r="CJ4" t="inlineStr">
-        <is>
-          <t>150mg</t>
-        </is>
-      </c>
-      <c r="CK4" t="inlineStr"/>
-      <c r="CL4" t="inlineStr">
-        <is>
-          <t>VD-27440-17</t>
-        </is>
-      </c>
-      <c r="CM4" t="n">
-        <v>120</v>
-      </c>
-      <c r="CN4" t="inlineStr">
-        <is>
-          <t>Công ty cổ phần dược phẩm Đạt Vi Phú</t>
-        </is>
-      </c>
-      <c r="CO4" t="inlineStr">
-        <is>
-          <t>Việt Nam</t>
-        </is>
-      </c>
-      <c r="CP4" t="inlineStr">
-        <is>
-          <t>Việt Nam</t>
-        </is>
-      </c>
-      <c r="CQ4" t="n">
-        <v>40.506</v>
-      </c>
-      <c r="CR4" t="inlineStr">
-        <is>
-          <t>Hatlop-150</t>
-        </is>
-      </c>
-      <c r="CS4" t="n">
-        <v>100</v>
-      </c>
-      <c r="CT4" t="n">
-        <v>855</v>
-      </c>
-      <c r="CU4" t="n">
-        <v>2</v>
-      </c>
-      <c r="CV4" t="inlineStr"/>
-      <c r="CW4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY4" t="n">
-        <v>2</v>
-      </c>
-      <c r="CZ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DA4" t="inlineStr">
-        <is>
-          <t>59/QĐ-TTMS</t>
-        </is>
-      </c>
-      <c r="DB4" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150) 150mg</t>
-        </is>
-      </c>
-      <c r="DC4" t="inlineStr"/>
-      <c r="DD4" t="inlineStr"/>
-      <c r="DE4" t="inlineStr">
-        <is>
-          <t>Irbesartan (Irbesartan (Hatlop-150)), 150mg</t>
-        </is>
-      </c>
-      <c r="DF4" t="b">
-        <v>1</v>
-      </c>
-      <c r="DG4" t="n">
-        <v>2497</v>
-      </c>
-      <c r="DH4" t="n">
-        <v>855</v>
-      </c>
-      <c r="DI4" t="inlineStr">
-        <is>
-          <t>Thuộc danh mục bảo hiểm chi</t>
-        </is>
-      </c>
-      <c r="DJ4" t="b">
-        <v>0</v>
-      </c>
-      <c r="DK4" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL4" t="inlineStr"/>
-      <c r="DM4" t="inlineStr"/>
-      <c r="DN4" t="inlineStr"/>
-      <c r="DO4" t="inlineStr"/>
-      <c r="DP4" t="inlineStr"/>
-      <c r="DQ4" t="inlineStr"/>
-      <c r="DR4" t="inlineStr"/>
-      <c r="DS4" t="inlineStr">
-        <is>
-          <t>Trưa: 1 Viên- Chiều: 1 Viên</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>3839</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>2</v>
-      </c>
-      <c r="N5" t="n">
-        <v>17437</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Quách Bảo Hưng</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="n">
-        <v>4803</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>knt1</t>
-        </is>
-      </c>
-      <c r="S5" t="n">
-        <v>13</v>
-      </c>
-      <c r="T5" t="n">
-        <v>13</v>
-      </c>
-      <c r="U5" t="n">
-        <v>30</v>
-      </c>
-      <c r="V5" t="n">
-        <v>130</v>
-      </c>
-      <c r="W5" t="n">
-        <v>2</v>
-      </c>
-      <c r="X5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>Lần</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Khám Nội Tiết 1</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>Khám Nội tiết</t>
-        </is>
-      </c>
-      <c r="AB5" t="n">
-        <v>1024</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>7.1897</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>1083660</v>
-      </c>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>17437|983307|149|10/05/2024 01:02|A00.9|Bệnh tả, không đặc hiệu|3839|3|10/05/2024 01:02|3839||||PendingProcessing|4803|80||Bệnh tả, không đặc hiệu|2|1083660|13||</t>
-        </is>
-      </c>
-      <c r="AL5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>28</v>
-      </c>
-      <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="inlineStr"/>
-      <c r="AP5" t="n">
-        <v>9843</v>
-      </c>
-      <c r="AQ5" t="inlineStr"/>
-      <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV5" t="inlineStr"/>
-      <c r="AW5" t="inlineStr"/>
-      <c r="AX5" t="inlineStr"/>
-      <c r="AY5" t="inlineStr"/>
-      <c r="AZ5" t="inlineStr"/>
-      <c r="BA5" t="inlineStr"/>
-      <c r="BB5" t="inlineStr"/>
-      <c r="BC5" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150) 150mg</t>
-        </is>
-      </c>
-      <c r="BD5" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="BE5" t="n">
-        <v>2</v>
-      </c>
-      <c r="BF5" t="inlineStr"/>
-      <c r="BG5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>127</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>5</v>
-      </c>
-      <c r="BN5" t="b">
-        <v>0</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP5" t="inlineStr">
-        <is>
-          <t>150mg</t>
-        </is>
-      </c>
-      <c r="BQ5" t="inlineStr">
-        <is>
-          <t>Uống</t>
-        </is>
-      </c>
-      <c r="BR5" t="inlineStr"/>
-      <c r="BS5" t="inlineStr">
-        <is>
-          <t>IrbT26</t>
-        </is>
-      </c>
-      <c r="BT5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU5" t="n">
-        <v>43</v>
-      </c>
-      <c r="BV5" t="inlineStr"/>
-      <c r="BW5" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150)</t>
-        </is>
-      </c>
-      <c r="BX5" t="inlineStr"/>
-      <c r="BY5" t="n">
-        <v>40.506</v>
-      </c>
-      <c r="BZ5" t="inlineStr">
-        <is>
-          <t>Hatlop-150</t>
-        </is>
-      </c>
-      <c r="CA5" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="CB5" t="inlineStr">
-        <is>
-          <t>Hộp</t>
-        </is>
-      </c>
-      <c r="CC5" t="inlineStr">
-        <is>
-          <t>Hộp</t>
-        </is>
-      </c>
-      <c r="CD5" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="CE5" t="n">
-        <v>100</v>
-      </c>
-      <c r="CF5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CG5" t="inlineStr">
-        <is>
-          <t>Irbesartan</t>
-        </is>
-      </c>
-      <c r="CH5" t="n">
-        <v>101</v>
-      </c>
-      <c r="CI5" t="n">
-        <v>101</v>
-      </c>
-      <c r="CJ5" t="inlineStr">
-        <is>
-          <t>150mg</t>
-        </is>
-      </c>
-      <c r="CK5" t="inlineStr"/>
-      <c r="CL5" t="inlineStr">
-        <is>
-          <t>VD-27440-17</t>
-        </is>
-      </c>
-      <c r="CM5" t="n">
-        <v>120</v>
-      </c>
-      <c r="CN5" t="inlineStr">
-        <is>
-          <t>Công ty cổ phần dược phẩm Đạt Vi Phú</t>
-        </is>
-      </c>
-      <c r="CO5" t="inlineStr">
-        <is>
-          <t>Việt Nam</t>
-        </is>
-      </c>
-      <c r="CP5" t="inlineStr">
-        <is>
-          <t>Việt Nam</t>
-        </is>
-      </c>
-      <c r="CQ5" t="n">
-        <v>40.506</v>
-      </c>
-      <c r="CR5" t="inlineStr">
-        <is>
-          <t>Hatlop-150</t>
-        </is>
-      </c>
-      <c r="CS5" t="n">
-        <v>100</v>
-      </c>
-      <c r="CT5" t="n">
-        <v>855</v>
-      </c>
-      <c r="CU5" t="n">
-        <v>2</v>
-      </c>
-      <c r="CV5" t="inlineStr"/>
-      <c r="CW5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY5" t="n">
-        <v>2</v>
-      </c>
-      <c r="CZ5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DA5" t="inlineStr">
-        <is>
-          <t>59/QĐ-TTMS</t>
-        </is>
-      </c>
-      <c r="DB5" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150) 150mg</t>
-        </is>
-      </c>
-      <c r="DC5" t="inlineStr"/>
-      <c r="DD5" t="inlineStr"/>
-      <c r="DE5" t="inlineStr">
-        <is>
-          <t>Irbesartan (Irbesartan (Hatlop-150)), 150mg</t>
-        </is>
-      </c>
-      <c r="DF5" t="b">
-        <v>1</v>
-      </c>
-      <c r="DG5" t="n">
-        <v>2497</v>
-      </c>
-      <c r="DH5" t="n">
-        <v>855</v>
-      </c>
-      <c r="DI5" t="inlineStr">
-        <is>
-          <t>Thuộc danh mục bảo hiểm chi</t>
-        </is>
-      </c>
-      <c r="DJ5" t="b">
-        <v>0</v>
-      </c>
-      <c r="DK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL5" t="inlineStr"/>
-      <c r="DM5" t="inlineStr"/>
-      <c r="DN5" t="inlineStr"/>
-      <c r="DO5" t="inlineStr"/>
-      <c r="DP5" t="inlineStr"/>
-      <c r="DQ5" t="inlineStr"/>
-      <c r="DR5" t="inlineStr"/>
-      <c r="DS5" t="inlineStr">
-        <is>
-          <t>Trưa: 1 Viên- Chiều: 1 Viên</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>3839</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>17437</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Quách Bảo Hưng</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="n">
-        <v>4803</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>knt1</t>
-        </is>
-      </c>
-      <c r="S6" t="n">
-        <v>13</v>
-      </c>
-      <c r="T6" t="n">
-        <v>13</v>
-      </c>
-      <c r="U6" t="n">
-        <v>30</v>
-      </c>
-      <c r="V6" t="n">
-        <v>130</v>
-      </c>
-      <c r="W6" t="n">
-        <v>2</v>
-      </c>
-      <c r="X6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Lần</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Khám Nội Tiết 1</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>Khám Nội tiết</t>
-        </is>
-      </c>
-      <c r="AB6" t="n">
-        <v>1024</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>7.1897</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>1083660</v>
-      </c>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>17437|983307|149|10/05/2024 01:02|A00.9|Bệnh tả, không đặc hiệu|3839|3|10/05/2024 01:02|3839||||PendingProcessing|4803|80||Bệnh tả, không đặc hiệu|2|1083660|13||</t>
-        </is>
-      </c>
-      <c r="AL6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>28</v>
-      </c>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="n">
-        <v>9843</v>
-      </c>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV6" t="inlineStr"/>
-      <c r="AW6" t="inlineStr"/>
-      <c r="AX6" t="inlineStr"/>
-      <c r="AY6" t="inlineStr"/>
-      <c r="AZ6" t="inlineStr"/>
-      <c r="BA6" t="inlineStr"/>
-      <c r="BB6" t="inlineStr"/>
-      <c r="BC6" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150) 150mg</t>
-        </is>
-      </c>
-      <c r="BD6" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="BE6" t="n">
-        <v>2</v>
-      </c>
-      <c r="BF6" t="inlineStr"/>
-      <c r="BG6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BI6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>127</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>5</v>
-      </c>
-      <c r="BN6" t="b">
-        <v>0</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP6" t="inlineStr">
-        <is>
-          <t>150mg</t>
-        </is>
-      </c>
-      <c r="BQ6" t="inlineStr">
-        <is>
-          <t>Uống</t>
-        </is>
-      </c>
-      <c r="BR6" t="inlineStr"/>
-      <c r="BS6" t="inlineStr">
-        <is>
-          <t>IrbT26</t>
-        </is>
-      </c>
-      <c r="BT6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU6" t="n">
-        <v>43</v>
-      </c>
-      <c r="BV6" t="inlineStr"/>
-      <c r="BW6" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150)</t>
-        </is>
-      </c>
-      <c r="BX6" t="inlineStr"/>
-      <c r="BY6" t="n">
-        <v>40.506</v>
-      </c>
-      <c r="BZ6" t="inlineStr">
-        <is>
-          <t>Hatlop-150</t>
-        </is>
-      </c>
-      <c r="CA6" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="CB6" t="inlineStr">
-        <is>
-          <t>Hộp</t>
-        </is>
-      </c>
-      <c r="CC6" t="inlineStr">
-        <is>
-          <t>Hộp</t>
-        </is>
-      </c>
-      <c r="CD6" t="inlineStr">
-        <is>
-          <t>Viên</t>
-        </is>
-      </c>
-      <c r="CE6" t="n">
-        <v>100</v>
-      </c>
-      <c r="CF6" t="n">
-        <v>1</v>
-      </c>
-      <c r="CG6" t="inlineStr">
-        <is>
-          <t>Irbesartan</t>
-        </is>
-      </c>
-      <c r="CH6" t="n">
-        <v>101</v>
-      </c>
-      <c r="CI6" t="n">
-        <v>101</v>
-      </c>
-      <c r="CJ6" t="inlineStr">
-        <is>
-          <t>150mg</t>
-        </is>
-      </c>
-      <c r="CK6" t="inlineStr"/>
-      <c r="CL6" t="inlineStr">
-        <is>
-          <t>VD-27440-17</t>
-        </is>
-      </c>
-      <c r="CM6" t="n">
-        <v>120</v>
-      </c>
-      <c r="CN6" t="inlineStr">
-        <is>
-          <t>Công ty cổ phần dược phẩm Đạt Vi Phú</t>
-        </is>
-      </c>
-      <c r="CO6" t="inlineStr">
-        <is>
-          <t>Việt Nam</t>
-        </is>
-      </c>
-      <c r="CP6" t="inlineStr">
-        <is>
-          <t>Việt Nam</t>
-        </is>
-      </c>
-      <c r="CQ6" t="n">
-        <v>40.506</v>
-      </c>
-      <c r="CR6" t="inlineStr">
-        <is>
-          <t>Hatlop-150</t>
-        </is>
-      </c>
-      <c r="CS6" t="n">
-        <v>100</v>
-      </c>
-      <c r="CT6" t="n">
-        <v>855</v>
-      </c>
-      <c r="CU6" t="n">
-        <v>2</v>
-      </c>
-      <c r="CV6" t="inlineStr"/>
-      <c r="CW6" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX6" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY6" t="n">
-        <v>2</v>
-      </c>
-      <c r="CZ6" t="n">
-        <v>1</v>
-      </c>
-      <c r="DA6" t="inlineStr">
-        <is>
-          <t>59/QĐ-TTMS</t>
-        </is>
-      </c>
-      <c r="DB6" t="inlineStr">
-        <is>
-          <t>Irbesartan (Hatlop-150) 150mg</t>
-        </is>
-      </c>
-      <c r="DC6" t="inlineStr"/>
-      <c r="DD6" t="inlineStr"/>
-      <c r="DE6" t="inlineStr">
-        <is>
-          <t>Irbesartan (Irbesartan (Hatlop-150)), 150mg</t>
-        </is>
-      </c>
-      <c r="DF6" t="b">
-        <v>1</v>
-      </c>
-      <c r="DG6" t="n">
-        <v>2497</v>
-      </c>
-      <c r="DH6" t="n">
-        <v>855</v>
-      </c>
-      <c r="DI6" t="inlineStr">
-        <is>
-          <t>Thuộc danh mục bảo hiểm chi</t>
-        </is>
-      </c>
-      <c r="DJ6" t="b">
-        <v>0</v>
-      </c>
-      <c r="DK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL6" t="inlineStr"/>
-      <c r="DM6" t="inlineStr"/>
-      <c r="DN6" t="inlineStr"/>
-      <c r="DO6" t="inlineStr"/>
-      <c r="DP6" t="inlineStr"/>
-      <c r="DQ6" t="inlineStr"/>
-      <c r="DR6" t="inlineStr"/>
-      <c r="DS6" t="inlineStr">
-        <is>
-          <t>Trưa: 1 Viên- Chiều: 1 Viên</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>